<commit_message>
Ajuste do nome das universidades.
</commit_message>
<xml_diff>
--- a/Contatos/Contatos.xlsx
+++ b/Contatos/Contatos.xlsx
@@ -39,15 +39,9 @@
     <t>Site</t>
   </si>
   <si>
-    <t>UNILAB</t>
-  </si>
-  <si>
     <t>historia.ba@unilab.edu.br</t>
   </si>
   <si>
-    <t>UFBA</t>
-  </si>
-  <si>
     <t>fch07@ufba.br</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t xml:space="preserve">Madalena Alcantara </t>
   </si>
   <si>
-    <t>UNEB/ SALVADOR</t>
-  </si>
-  <si>
     <t>colegiadohistoria6@gmail.com</t>
   </si>
   <si>
@@ -84,9 +75,6 @@
     <t>Juliano Silva</t>
   </si>
   <si>
-    <t>UNEB/ALAGOINHAS</t>
-  </si>
-  <si>
     <t>colegiado.historia@yahoo.com.br</t>
   </si>
   <si>
@@ -105,18 +93,12 @@
     <t>Uilma Santos</t>
   </si>
   <si>
-    <t>UNEB/JACOBINA</t>
-  </si>
-  <si>
     <t>historiadch4@uneb.br</t>
   </si>
   <si>
     <t>(74) 3621-3337 (Ramal 225)</t>
   </si>
   <si>
-    <t>UNEB / TEIXIERA DE FREITAS</t>
-  </si>
-  <si>
     <t>jonathanmolar@hotmail.com - colegiadodehistoria2012@gmail.com</t>
   </si>
   <si>
@@ -129,9 +111,6 @@
     <t>Frederico Loiola Viana</t>
   </si>
   <si>
-    <t>UNEB/ ITABERABA</t>
-  </si>
-  <si>
     <t>laslima@uneb.br</t>
   </si>
   <si>
@@ -150,9 +129,6 @@
     <t>https://www.ufsb.edu.br/cfchs/graduacao/historia</t>
   </si>
   <si>
-    <t>UFRB</t>
-  </si>
-  <si>
     <t>Seg/Sex. 8h às 12h</t>
   </si>
   <si>
@@ -189,18 +165,9 @@
     <t>https://portal.uneb.br/eunapolis/cursos/historia</t>
   </si>
   <si>
-    <t>UNEB/ EUNÁPOLIS</t>
-  </si>
-  <si>
-    <t>UNEB/ CAETITÉ</t>
-  </si>
-  <si>
     <t>Cleidiane Silva Araújo</t>
   </si>
   <si>
-    <t>UNEB/CONCEIÇÃO DO COITÉ</t>
-  </si>
-  <si>
     <t>https://portal.uneb.br/itaberaba/cursos/historia</t>
   </si>
   <si>
@@ -313,6 +280,39 @@
   </si>
   <si>
     <t>__</t>
+  </si>
+  <si>
+    <t>Universidade da Integração Internacional da Lusofonia Afro-Brasileira - UNILAB</t>
+  </si>
+  <si>
+    <t>Universidade Federal da Bahia -UFBA</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/ SALVADOR</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/ CAETITÉ</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/ALAGOINHAS</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/CONCEIÇÃO DO COITÉ</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/JACOBINA</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB / TEIXIERA DE FREITAS</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/ ITABERABA</t>
+  </si>
+  <si>
+    <t>Universidade do Estado da Bahia - UNEB/ EUNÁPOLIS</t>
+  </si>
+  <si>
+    <t>Universidade Federal do Recôncavo Baiano - UFRB</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
@@ -852,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1177,13 +1180,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="63" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.140625" style="8" bestFit="1" customWidth="1"/>
@@ -1193,7 +1196,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1203,7 +1206,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1215,369 +1218,369 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
+      <c r="A5" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
+      <c r="A10" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
+      <c r="A11" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>70</v>
+      <c r="A12" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>72</v>
+      <c r="A14" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>73</v>
+      <c r="A15" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>74</v>
+      <c r="A16" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
+      <c r="A17" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>